<commit_message>
Sprague uBiome data from April 2015
allows for A/B comparison because the samples are one week apart.
</commit_message>
<xml_diff>
--- a/Data/sprague data/Sprague MFP Macronutrients Apr Test Period 2015.xlsx
+++ b/Data/sprague data/Sprague MFP Macronutrients Apr Test Period 2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Sprague\OneDrive\Projects\Programming\uBiome\Data\sprague data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Sprague\OneDrive\Projects\uBiome\Data\sprague data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="MyFitnessPal_Food_Data_Export(0" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -72,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -570,7 +570,7 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2141,35 +2141,35 @@
         <v>11</v>
       </c>
       <c r="B44" s="2">
-        <f>AVERAGE(B2:B42)</f>
+        <f t="shared" ref="B44:I44" si="0">AVERAGE(B2:B42)</f>
         <v>1841.7073170731708</v>
       </c>
       <c r="C44" s="2">
-        <f>AVERAGE(C2:C42)</f>
+        <f t="shared" si="0"/>
         <v>192.17073170731706</v>
       </c>
       <c r="D44" s="2">
-        <f>AVERAGE(D2:D42)</f>
+        <f t="shared" si="0"/>
         <v>102.6829268292683</v>
       </c>
       <c r="E44" s="2">
-        <f>AVERAGE(E2:E42)</f>
+        <f t="shared" si="0"/>
         <v>94.853658536585371</v>
       </c>
       <c r="F44" s="2">
-        <f>AVERAGE(F2:F42)</f>
+        <f t="shared" si="0"/>
         <v>268</v>
       </c>
       <c r="G44" s="2">
-        <f>AVERAGE(G2:G42)</f>
+        <f t="shared" si="0"/>
         <v>2298.5365853658536</v>
       </c>
       <c r="H44" s="2">
-        <f>AVERAGE(H2:H42)</f>
+        <f t="shared" si="0"/>
         <v>64.121951219512198</v>
       </c>
       <c r="I44" s="2">
-        <f>AVERAGE(I2:I42)</f>
+        <f t="shared" si="0"/>
         <v>15.219512195121951</v>
       </c>
     </row>
@@ -2182,31 +2182,31 @@
         <v>2242.5714285714284</v>
       </c>
       <c r="C45" s="2">
-        <f t="shared" ref="C45:I45" si="0">AVERAGE(C22:C28)</f>
+        <f t="shared" ref="C45:I45" si="1">AVERAGE(C22:C28)</f>
         <v>241.85714285714286</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124.71428571428571</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>108.71428571428571</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>262.28571428571428</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2814.2857142857142</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78.285714285714292</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.857142857142858</v>
       </c>
     </row>
@@ -2219,31 +2219,31 @@
         <v>400.86411149825767</v>
       </c>
       <c r="C46" s="2">
-        <f t="shared" ref="C46:I46" si="1">C45-C44</f>
+        <f t="shared" ref="C46:I46" si="2">C45-C44</f>
         <v>49.686411149825801</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22.031358885017411</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.860627177700337</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.7142857142857224</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>515.7491289198606</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.163763066202094</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6376306620209071</v>
       </c>
     </row>
@@ -2256,31 +2256,31 @@
         <v>1.2176589666458557</v>
       </c>
       <c r="C47" s="6">
-        <f t="shared" ref="C47:I47" si="2">C45/C44</f>
+        <f t="shared" ref="C47:I47" si="3">C45/C44</f>
         <v>1.2585534785052492</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2145571767899557</v>
       </c>
       <c r="E47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1461264372038349</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97867803837953093</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2243815183119089</v>
       </c>
       <c r="H47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2208878987121665</v>
       </c>
       <c r="I47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1076007326007327</v>
       </c>
     </row>

</xml_diff>